<commit_message>
* Logging adjustments. * Test fixes - they used dynamic dates which could not be tested. * Addition of 'exception' and 'type' attributes to sql node.
</commit_message>
<xml_diff>
--- a/tests/data/desired/datetimereport.xlsx
+++ b/tests/data/desired/datetimereport.xlsx
@@ -143,7 +143,7 @@
         <v>40897.458333333336</v>
       </c>
       <c r="C2" t="n" s="3">
-        <v>40867.0</v>
+        <v>40848.0</v>
       </c>
       <c r="D2" t="n" s="4">
         <v>25569.0</v>
@@ -157,7 +157,7 @@
         <v>40897.45903935185</v>
       </c>
       <c r="C3" t="n" s="3">
-        <v>40867.0</v>
+        <v>40849.0</v>
       </c>
       <c r="D3" t="n" s="4">
         <v>25569.042372685184</v>
@@ -171,7 +171,7 @@
         <v>40897.45974537037</v>
       </c>
       <c r="C4" t="n" s="3">
-        <v>40867.0</v>
+        <v>40850.0</v>
       </c>
       <c r="D4" t="n" s="4">
         <v>25569.084745370372</v>
@@ -185,7 +185,7 @@
         <v>40897.46045138889</v>
       </c>
       <c r="C5" t="n" s="3">
-        <v>40867.0</v>
+        <v>40851.0</v>
       </c>
       <c r="D5" t="n" s="4">
         <v>25569.127118055556</v>
@@ -199,7 +199,7 @@
         <v>40897.46115740741</v>
       </c>
       <c r="C6" t="n" s="3">
-        <v>40867.0</v>
+        <v>40852.0</v>
       </c>
       <c r="D6" t="n" s="4">
         <v>25569.16949074074</v>
@@ -213,7 +213,7 @@
         <v>40897.461863425924</v>
       </c>
       <c r="C7" t="n" s="3">
-        <v>40867.0</v>
+        <v>40853.0</v>
       </c>
       <c r="D7" t="n" s="4">
         <v>25569.211863425928</v>
@@ -227,7 +227,7 @@
         <v>40897.46256944445</v>
       </c>
       <c r="C8" t="n" s="3">
-        <v>40867.0</v>
+        <v>40854.0</v>
       </c>
       <c r="D8" t="n" s="4">
         <v>25569.254236111112</v>
@@ -241,7 +241,7 @@
         <v>40897.463275462964</v>
       </c>
       <c r="C9" t="n" s="3">
-        <v>40867.0</v>
+        <v>40855.0</v>
       </c>
       <c r="D9" t="n" s="4">
         <v>25569.296608796296</v>
@@ -255,7 +255,7 @@
         <v>40897.46398148148</v>
       </c>
       <c r="C10" t="n" s="3">
-        <v>40867.0</v>
+        <v>40856.0</v>
       </c>
       <c r="D10" t="n" s="4">
         <v>25569.33898148148</v>
@@ -269,7 +269,7 @@
         <v>40897.4646875</v>
       </c>
       <c r="C11" t="n" s="3">
-        <v>40867.0</v>
+        <v>40857.0</v>
       </c>
       <c r="D11" t="n" s="4">
         <v>25569.381354166668</v>
@@ -283,7 +283,7 @@
         <v>40897.46539351852</v>
       </c>
       <c r="C12" t="n" s="3">
-        <v>40867.0</v>
+        <v>40858.0</v>
       </c>
       <c r="D12" t="n" s="4">
         <v>25569.423726851852</v>
@@ -297,7 +297,7 @@
         <v>40897.466099537036</v>
       </c>
       <c r="C13" t="n" s="3">
-        <v>40867.0</v>
+        <v>40859.0</v>
       </c>
       <c r="D13" t="n" s="4">
         <v>25569.466099537036</v>
@@ -311,7 +311,7 @@
         <v>40897.46680555555</v>
       </c>
       <c r="C14" t="n" s="3">
-        <v>40867.0</v>
+        <v>40860.0</v>
       </c>
       <c r="D14" t="n" s="4">
         <v>25569.508472222224</v>
@@ -325,7 +325,7 @@
         <v>40897.467511574076</v>
       </c>
       <c r="C15" t="n" s="3">
-        <v>40867.0</v>
+        <v>40861.0</v>
       </c>
       <c r="D15" t="n" s="4">
         <v>25569.550844907408</v>
@@ -339,7 +339,7 @@
         <v>40897.46821759259</v>
       </c>
       <c r="C16" t="n" s="3">
-        <v>40867.0</v>
+        <v>40862.0</v>
       </c>
       <c r="D16" t="n" s="4">
         <v>25569.593217592592</v>
@@ -353,7 +353,7 @@
         <v>40897.46892361111</v>
       </c>
       <c r="C17" t="n" s="3">
-        <v>40867.0</v>
+        <v>40863.0</v>
       </c>
       <c r="D17" t="n" s="4">
         <v>25569.63559027778</v>
@@ -367,7 +367,7 @@
         <v>40897.46962962963</v>
       </c>
       <c r="C18" t="n" s="3">
-        <v>40867.0</v>
+        <v>40864.0</v>
       </c>
       <c r="D18" t="n" s="4">
         <v>25569.677962962964</v>
@@ -381,7 +381,7 @@
         <v>40897.47033564815</v>
       </c>
       <c r="C19" t="n" s="3">
-        <v>40867.0</v>
+        <v>40865.0</v>
       </c>
       <c r="D19" t="n" s="4">
         <v>25569.720335648148</v>
@@ -395,7 +395,7 @@
         <v>40897.471041666664</v>
       </c>
       <c r="C20" t="n" s="3">
-        <v>40867.0</v>
+        <v>40866.0</v>
       </c>
       <c r="D20" t="n" s="4">
         <v>25569.762708333332</v>

</xml_diff>